<commit_message>
feat: Melhorias na gestão de jogos
- Restrição de alterações em times apenas para jogos agendados
- URL dinâmica para confirmação de presença baseada no ambiente
- Atualização do .gitignore para arquivos sensíveis
</commit_message>
<xml_diff>
--- a/Historico de versoes.xlsx
+++ b/Historico de versoes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IvoDados\futconnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8D1522-083B-45C5-88B9-53460B6C137C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFFD705-450D-43B1-8EB7-8DCA6BBE06B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41460" yWindow="840" windowWidth="19200" windowHeight="11175" xr2:uid="{006592B2-3030-4BC1-84EF-C04048D4560E}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{006592B2-3030-4BC1-84EF-C04048D4560E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Histórico de versões do Futconnect</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Implantando politicas no financeiro e mensalidades.</t>
+  </si>
+  <si>
+    <t>Futconnect2703 1619</t>
+  </si>
+  <si>
+    <t>Politicas em mensalidades, jogos e sócios - feito o commit</t>
   </si>
 </sst>
 </file>
@@ -443,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92DE2D2-EFA7-4D5E-A4BD-0E2FC4950F88}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,6 +520,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>45743</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.67986111111111114</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
filtro de data no dash e ajuste de formulas
</commit_message>
<xml_diff>
--- a/Historico de versoes.xlsx
+++ b/Historico de versoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IvoDados\futconnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BEB7B4-4442-47CD-AB24-D40B8E105438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7085124C-7508-4775-9CEE-3F160FB41D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{006592B2-3030-4BC1-84EF-C04048D4560E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Histórico de versões do Futconnect</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>Arrumado transação.</t>
+  </si>
+  <si>
+    <t>Futconnect 3103 0900</t>
+  </si>
+  <si>
+    <t>Arrumado estatisticas do jogo quando jogador cancela participação</t>
   </si>
 </sst>
 </file>
@@ -473,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92DE2D2-EFA7-4D5E-A4BD-0E2FC4950F88}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -614,6 +620,20 @@
         <v>19</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>45747</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
ajuste no modal estatistica e valor no dash
</commit_message>
<xml_diff>
--- a/Historico de versoes.xlsx
+++ b/Historico de versoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IvoDados\futconnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7085124C-7508-4775-9CEE-3F160FB41D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CF2754-C3D6-4A8C-8CFB-3D6481600975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{006592B2-3030-4BC1-84EF-C04048D4560E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Histórico de versões do Futconnect</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Arrumado estatisticas do jogo quando jogador cancela participação</t>
+  </si>
+  <si>
+    <t>Futconnect 3103 1017</t>
+  </si>
+  <si>
+    <t>Implantado filtro de ano no dash e corrigido fórmula da participação.</t>
   </si>
 </sst>
 </file>
@@ -479,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92DE2D2-EFA7-4D5E-A4BD-0E2FC4950F88}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,6 +640,20 @@
         <v>21</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>45747</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
melhora carregamento pag socios
</commit_message>
<xml_diff>
--- a/Historico de versoes.xlsx
+++ b/Historico de versoes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IvoDados\futconnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A00A29-B581-492B-A2D5-3FC3A82DB7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FDC712-50B5-44BF-966D-B206FBA57840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{006592B2-3030-4BC1-84EF-C04048D4560E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{006592B2-3030-4BC1-84EF-C04048D4560E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Histórico de versões do Futconnect</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Ajuste nas estatisticas do jogador, criado documentos e ajuste na gravação das configurações</t>
+  </si>
+  <si>
+    <t>Futconnect0304 0950</t>
+  </si>
+  <si>
+    <t>Responsividade das páginas.</t>
   </si>
 </sst>
 </file>
@@ -491,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92DE2D2-EFA7-4D5E-A4BD-0E2FC4950F88}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -674,6 +680,20 @@
         <v>25</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>45750</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.40972222222222221</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
filtro de datas em movimentacoes
</commit_message>
<xml_diff>
--- a/Historico de versoes.xlsx
+++ b/Historico de versoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IvoDados\futconnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FDC712-50B5-44BF-966D-B206FBA57840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539EB93C-3432-452D-923D-4B19564CCF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{006592B2-3030-4BC1-84EF-C04048D4560E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Histórico de versões do Futconnect</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Responsividade das páginas.</t>
+  </si>
+  <si>
+    <t>Futconnect0404 1900</t>
+  </si>
+  <si>
+    <t>Ajustes nos filtros de datas e no apelido e email ao cadastro um novo sócio.</t>
   </si>
 </sst>
 </file>
@@ -497,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92DE2D2-EFA7-4D5E-A4BD-0E2FC4950F88}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -694,6 +700,20 @@
         <v>27</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>45751</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
melhora na pagina movimentacoes
</commit_message>
<xml_diff>
--- a/Historico de versoes.xlsx
+++ b/Historico de versoes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IvoDados\futconnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539EB93C-3432-452D-923D-4B19564CCF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1311D83-0C4F-42AC-B8F7-957F8071C4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{006592B2-3030-4BC1-84EF-C04048D4560E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Histórico de versões do Futconnect</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>Ajustes nos filtros de datas e no apelido e email ao cadastro um novo sócio.</t>
+  </si>
+  <si>
+    <t>Futconnect0904 1514</t>
+  </si>
+  <si>
+    <t>Manual, participação efetiva e filtros nas abas de performance.</t>
   </si>
 </sst>
 </file>
@@ -503,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92DE2D2-EFA7-4D5E-A4BD-0E2FC4950F88}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -714,6 +720,20 @@
         <v>29</v>
       </c>
     </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>45756</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.63472222222222219</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>